<commit_message>
update the template sheet
</commit_message>
<xml_diff>
--- a/Leaves_Petals/metadata collection sheet template.xlsx
+++ b/Leaves_Petals/metadata collection sheet template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dena/Documents/GitHub/health-ri-metadata/Leaves_Petals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619CFFC3-151B-B349-AE9B-5169230CC3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003E8CDD-3D2A-874E-A0CB-221E8CF6A650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="1620" windowWidth="26840" windowHeight="15940" xr2:uid="{A874C97F-E3B0-7D43-AEF0-908EBA91F58B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>description</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>values</t>
+  </si>
+  <si>
+    <t>target element from (your domain standards)</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3765D7B8-07BE-F149-87ED-9544B7AF89EC}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,7 +448,7 @@
     <col min="6" max="6" width="39.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -463,6 +466,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DCAT-AP folder is added
</commit_message>
<xml_diff>
--- a/Leaves_Petals/metadata collection sheet template.xlsx
+++ b/Leaves_Petals/metadata collection sheet template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dena/Documents/GitHub/health-ri-metadata/Leaves_Petals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003E8CDD-3D2A-874E-A0CB-221E8CF6A650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F22E27-2E44-6B4C-AB3A-D35437D28AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="1620" windowWidth="26840" windowHeight="15940" xr2:uid="{A874C97F-E3B0-7D43-AEF0-908EBA91F58B}"/>
   </bookViews>
@@ -434,18 +434,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3765D7B8-07BE-F149-87ED-9544B7AF89EC}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
     <col min="4" max="4" width="39.1640625" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="39.83203125" customWidth="1"/>
+    <col min="7" max="7" width="56.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.2">

</xml_diff>